<commit_message>
add white box test and telegram fee test and add ui text part
</commit_message>
<xml_diff>
--- a/src/main/resources/calendarTestCases.xlsx
+++ b/src/main/resources/calendarTestCases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382D488F-99DC-4758-844B-7584DEE62712}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65E4FF2-3CE8-46AE-A0AF-97E6B81FD7E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="26">
   <si>
     <t>测试用例编号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -80,12 +80,46 @@
   <si>
     <t>2100年3月1日</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1993年3月21日</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>1919年9月30日</t>
+  </si>
+  <si>
+    <t>2004年2月29日</t>
+  </si>
+  <si>
+    <t>2008年10月31日</t>
+  </si>
+  <si>
+    <t>2001年1月1日</t>
+  </si>
+  <si>
+    <t>2017年3月1日</t>
+  </si>
+  <si>
+    <t>日期不符合规则</t>
+  </si>
+  <si>
+    <t>2100年2月29日</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>2100年3月1日</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -408,13 +442,13 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="23" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -456,6 +490,12 @@
       <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -473,6 +513,12 @@
       <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -490,6 +536,12 @@
       <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -507,6 +559,12 @@
       <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -524,6 +582,12 @@
       <c r="E6" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -541,6 +605,12 @@
       <c r="E7" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -558,6 +628,12 @@
       <c r="E8" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -575,6 +651,12 @@
       <c r="E9" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -592,6 +674,12 @@
       <c r="E10" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -609,6 +697,12 @@
       <c r="E11" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -625,6 +719,12 @@
       </c>
       <c r="E12" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clean the execute data
</commit_message>
<xml_diff>
--- a/src/main/resources/calendarTestCases.xlsx
+++ b/src/main/resources/calendarTestCases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65E4FF2-3CE8-46AE-A0AF-97E6B81FD7E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017534EC-5DF5-4EE4-BAE6-B490BBB42291}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>测试用例编号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -80,46 +80,12 @@
   <si>
     <t>2100年3月1日</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1993年3月21日</t>
-  </si>
-  <si>
-    <t>pass</t>
-  </si>
-  <si>
-    <t>1919年9月30日</t>
-  </si>
-  <si>
-    <t>2004年2月29日</t>
-  </si>
-  <si>
-    <t>2008年10月31日</t>
-  </si>
-  <si>
-    <t>2001年1月1日</t>
-  </si>
-  <si>
-    <t>2017年3月1日</t>
-  </si>
-  <si>
-    <t>日期不符合规则</t>
-  </si>
-  <si>
-    <t>2100年2月29日</t>
-  </si>
-  <si>
-    <t>fail</t>
-  </si>
-  <si>
-    <t>2100年3月1日</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -442,13 +408,13 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="5" max="5" width="23" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -490,12 +456,6 @@
       <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -513,12 +473,6 @@
       <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -536,12 +490,6 @@
       <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -559,12 +507,6 @@
       <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -582,12 +524,6 @@
       <c r="E6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -605,12 +541,6 @@
       <c r="E7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -628,12 +558,6 @@
       <c r="E8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -651,12 +575,6 @@
       <c r="E9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -674,12 +592,6 @@
       <c r="E10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -697,12 +609,6 @@
       <c r="E11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -719,12 +625,6 @@
       </c>
       <c r="E12" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="F12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add test case design
</commit_message>
<xml_diff>
--- a/src/main/resources/calendarTestCases.xlsx
+++ b/src/main/resources/calendarTestCases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017534EC-5DF5-4EE4-BAE6-B490BBB42291}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C26A6D-28F4-45C0-8845-B9EFE8918D53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -408,7 +408,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>